<commit_message>
one to forty check website for domain price
</commit_message>
<xml_diff>
--- a/business/domain/domain-irnic-price-compare-list.xlsx
+++ b/business/domain/domain-irnic-price-compare-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web\projects\talambar_cdn\business\domain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\talambar_cdn\business\domain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2938B938-62EF-4768-A3D6-AD55C17031E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB99D3F-0C4F-4073-82FE-1D241BCA95C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{656E8D54-B9ED-4B19-91BC-7A9F1ADCF6AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{656E8D54-B9ED-4B19-91BC-7A9F1ADCF6AA}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="264">
   <si>
     <t>#</t>
   </si>
@@ -758,6 +758,66 @@
   </si>
   <si>
     <t>قرارداد سال</t>
+  </si>
+  <si>
+    <t>سایتش فعال نیست</t>
+  </si>
+  <si>
+    <t>دامنه بین المللی ندارد</t>
+  </si>
+  <si>
+    <t>دامنه بین المللی ندارد و شبیه بالا</t>
+  </si>
+  <si>
+    <t>دامنه بین المللی و پنج ساله IR ندارد</t>
+  </si>
+  <si>
+    <t>پنج ساله ندارد</t>
+  </si>
+  <si>
+    <t>com ندارد</t>
+  </si>
+  <si>
+    <t>تمدید 5 ساله ندارد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دامنه دات ای ار </t>
+  </si>
+  <si>
+    <t>دامنه ای ار 3100 تخفیف و دات کام 55000 تومان تخفیف</t>
+  </si>
+  <si>
+    <t>دامنه برای فروش ندارد</t>
+  </si>
+  <si>
+    <t>دامنه دات ای ار 8100 تخفیف دات کام 20000 تومان تخفیف</t>
+  </si>
+  <si>
+    <t>این نماینده در تاریخ 1400/1/14 فعالیتش به پایان رسید</t>
+  </si>
+  <si>
+    <t>دامنه دات کام برای فروش ندارد</t>
+  </si>
+  <si>
+    <t>دامنه دات کام 10000 تخفیف و دامنه دات ای ار ندارد</t>
+  </si>
+  <si>
+    <t>دامنه پنج ساله ندارد</t>
+  </si>
+  <si>
+    <t>برای فروش نیست</t>
+  </si>
+  <si>
+    <t>دامنه دات کام قیمت نداشت</t>
+  </si>
+  <si>
+    <t>سایت ندارد</t>
+  </si>
+  <si>
+    <t>سرویس فروش دامنه قطع بود</t>
+  </si>
+  <si>
+    <t>مشکل در لاگین و نبود تعرفه ها</t>
   </si>
 </sst>
 </file>
@@ -766,20 +826,20 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -787,7 +847,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -888,7 +948,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -930,7 +990,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -940,8 +1000,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -985,7 +1052,7 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
+      <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
     </dxf>
     <dxf>
       <font>
@@ -1022,11 +1089,8 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1045,8 +1109,51 @@
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Dana"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Dana"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1084,14 +1191,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Dana"/>
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1104,14 +1216,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
         <name val="Dana"/>
         <charset val="178"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1161,76 +1278,14 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Dana"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Dana"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Dana"/>
-        <charset val="178"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FFFFFFFF"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1251,11 +1306,23 @@
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color rgb="FFFFFFFF"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Dana"/>
+        <charset val="178"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5973,18 +6040,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{548BE326-327C-454C-ACE6-EB8CB003DD8D}" name="Table1" displayName="Table1" ref="A1:J78" totalsRowShown="0" headerRowDxfId="12" dataDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{548BE326-327C-454C-ACE6-EB8CB003DD8D}" name="Table1" displayName="Table1" ref="A1:J78" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:J78" xr:uid="{548BE326-327C-454C-ACE6-EB8CB003DD8D}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{2A23BA31-9B49-4E05-BE22-9FA47E3CF962}" name="#" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{64709FED-287E-48BA-9FE1-08622E4296D3}" name="شناسه" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{2A23BA31-9B49-4E05-BE22-9FA47E3CF962}" name="#" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{64709FED-287E-48BA-9FE1-08622E4296D3}" name="شناسه" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{C0E08190-D533-4D2F-AFDC-2037946ED136}" name="نام" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C2D57F2C-E391-415E-83DF-7489FFD9BBCC}" name="سامانه ثبت" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{8A8E354B-8721-44DE-AA34-4EEF648873E8}" name="وب" dataDxfId="6" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{68E090CB-E86E-4768-90BB-B4F444A7A9CD}" name="سایت فعال" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FBE5E785-E23D-4F5F-97F2-B7ED1FDF9ABA}" name="دامنه IR یکساله" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{730C9C40-D5E6-4344-97C0-C69019B1DC08}" name="دامنه IR پنج‌ساله" dataDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{BF2543EC-C8B4-4885-AFBB-1BBF36480F81}" name="دامنه دات‌کام" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{C2D57F2C-E391-415E-83DF-7489FFD9BBCC}" name="سامانه ثبت" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{8A8E354B-8721-44DE-AA34-4EEF648873E8}" name="وب" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{68E090CB-E86E-4768-90BB-B4F444A7A9CD}" name="سایت فعال" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{FBE5E785-E23D-4F5F-97F2-B7ED1FDF9ABA}" name="دامنه IR یکساله" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{730C9C40-D5E6-4344-97C0-C69019B1DC08}" name="دامنه IR پنج‌ساله" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{BF2543EC-C8B4-4885-AFBB-1BBF36480F81}" name="دامنه دات‌کام" dataDxfId="4" dataCellStyle="Comma"/>
     <tableColumn id="11" xr3:uid="{E6EFF9A6-1E16-4749-A354-9F03F60AD56E}" name="توضیح" dataDxfId="3" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6302,29 +6369,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B09669C-DC32-412C-96EB-9A29D963BFE0}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.875" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="10" max="10" width="36.25" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.125" style="1"/>
     <col min="15" max="15" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.75" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6356,7 +6423,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -6370,13 +6437,23 @@
       <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="19"/>
+      <c r="F2" s="18">
+        <v>5</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="18" customHeight="1">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6390,13 +6467,23 @@
       <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="19"/>
+      <c r="F3" s="18">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H3" s="15">
+        <v>48000</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="18" customHeight="1">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6408,13 +6495,23 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="19"/>
+      <c r="F4" s="18">
+        <v>10</v>
+      </c>
+      <c r="G4" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H4" s="15">
+        <v>48000</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="18" customHeight="1">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -6428,13 +6525,23 @@
       <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="19"/>
+      <c r="F5" s="18">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="18" customHeight="1">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -6448,13 +6555,23 @@
       <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="19"/>
+      <c r="F6" s="18">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="18" customHeight="1">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -6468,13 +6585,23 @@
       <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="19"/>
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="18" customHeight="1">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -6488,13 +6615,23 @@
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="19"/>
+      <c r="F8" s="18">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="18" customHeight="1">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -6508,13 +6645,23 @@
       <c r="E9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="19"/>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="18" customHeight="1">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -6525,16 +6672,26 @@
         <v>29</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="19"/>
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15">
+        <v>0</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="18" customHeight="1">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -6548,13 +6705,23 @@
       <c r="E11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="19"/>
+      <c r="F11" s="18">
+        <v>10</v>
+      </c>
+      <c r="G11" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15">
+        <v>285000</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="18" customHeight="1">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -6568,13 +6735,23 @@
       <c r="E12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="19"/>
+      <c r="F12" s="18">
+        <v>10</v>
+      </c>
+      <c r="G12" s="15">
+        <v>12900</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
+        <v>315000</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="18" customHeight="1">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -6588,13 +6765,23 @@
       <c r="E13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="19"/>
+      <c r="F13" s="18">
+        <v>10</v>
+      </c>
+      <c r="G13" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H13" s="15">
+        <v>48000</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="18" customHeight="1">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -6608,13 +6795,23 @@
       <c r="E14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="19"/>
+      <c r="F14" s="18">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15">
+        <v>13900</v>
+      </c>
+      <c r="H14" s="15">
+        <v>48000</v>
+      </c>
+      <c r="I14" s="15">
+        <v>338000</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="18" customHeight="1">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -6625,16 +6822,26 @@
         <v>44</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="19"/>
+      <c r="F15" s="18">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <v>12000</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="18" customHeight="1">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -6645,16 +6852,26 @@
         <v>47</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="19"/>
+      <c r="F16" s="18">
+        <v>10</v>
+      </c>
+      <c r="G16" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0</v>
+      </c>
+      <c r="I16" s="15">
+        <v>395000</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="18" customHeight="1">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -6668,13 +6885,23 @@
       <c r="E17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="19"/>
+      <c r="F17" s="18">
+        <v>5</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="18" customHeight="1">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -6688,13 +6915,23 @@
       <c r="E18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="19"/>
+      <c r="F18" s="18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="15">
+        <v>19000</v>
+      </c>
+      <c r="H18" s="15">
+        <v>57000</v>
+      </c>
+      <c r="I18" s="15">
+        <v>348000</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="18" customHeight="1">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -6705,16 +6942,26 @@
         <v>56</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="19"/>
+      <c r="F19" s="18">
+        <v>10</v>
+      </c>
+      <c r="G19" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0</v>
+      </c>
+      <c r="I19" s="15">
+        <v>365000</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>250</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" ht="18" customHeight="1">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -6728,13 +6975,23 @@
       <c r="E20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="19"/>
+      <c r="F20" s="18">
+        <v>0</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="18" customHeight="1">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -6748,13 +7005,23 @@
       <c r="E21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="19"/>
+      <c r="F21" s="18">
+        <v>0</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" ht="18" customHeight="1">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -6765,16 +7032,26 @@
         <v>65</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="19"/>
+      <c r="F22" s="18">
+        <v>5</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="18" customHeight="1">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -6788,13 +7065,23 @@
       <c r="E23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="19"/>
+      <c r="F23" s="18">
+        <v>10</v>
+      </c>
+      <c r="G23" s="15">
+        <v>16900</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0</v>
+      </c>
+      <c r="I23" s="15">
+        <v>279000</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" ht="18" customHeight="1">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -6808,13 +7095,23 @@
       <c r="E24" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="19"/>
+      <c r="F24" s="18">
+        <v>10</v>
+      </c>
+      <c r="G24" s="15">
+        <v>14940</v>
+      </c>
+      <c r="H24" s="15">
+        <v>45750</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" ht="18" customHeight="1">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -6828,13 +7125,21 @@
       <c r="E25" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="15"/>
+      <c r="F25" s="18">
+        <v>10</v>
+      </c>
+      <c r="G25" s="15">
+        <v>16000</v>
+      </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="19"/>
+      <c r="I25" s="15">
+        <v>298000</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" ht="18" customHeight="1">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -6848,13 +7153,23 @@
       <c r="E26" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="19"/>
+      <c r="F26" s="18">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="18" customHeight="1">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -6865,16 +7180,26 @@
         <v>80</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="19"/>
+      <c r="F27" s="18">
+        <v>10</v>
+      </c>
+      <c r="G27" s="15">
+        <v>12000</v>
+      </c>
+      <c r="H27" s="15">
+        <v>45000</v>
+      </c>
+      <c r="I27" s="15">
+        <v>0</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>256</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" ht="18" customHeight="1">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -6888,13 +7213,23 @@
       <c r="E28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="19"/>
+      <c r="F28" s="18">
+        <v>10</v>
+      </c>
+      <c r="G28" s="15">
+        <v>15000</v>
+      </c>
+      <c r="H28" s="15">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15">
+        <v>279000</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" ht="18" customHeight="1">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -6908,13 +7243,23 @@
       <c r="E29" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="19"/>
+      <c r="F29" s="18">
+        <v>5</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15">
+        <v>0</v>
+      </c>
+      <c r="I29" s="15">
+        <v>0</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>262</v>
+      </c>
     </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" ht="18" customHeight="1">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -6925,16 +7270,26 @@
         <v>89</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="19"/>
+      <c r="F30" s="18">
+        <v>10</v>
+      </c>
+      <c r="G30" s="15">
+        <v>14900</v>
+      </c>
+      <c r="H30" s="15">
+        <v>0</v>
+      </c>
+      <c r="I30" s="15">
+        <v>295000</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="31" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" ht="18" customHeight="1">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -6948,13 +7303,23 @@
       <c r="E31" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="19"/>
+      <c r="F31" s="18">
+        <v>10</v>
+      </c>
+      <c r="G31" s="15">
+        <v>16000</v>
+      </c>
+      <c r="H31" s="15">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
+        <v>310000</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>258</v>
+      </c>
     </row>
-    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" ht="18" customHeight="1">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -6968,13 +7333,23 @@
       <c r="E32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="19"/>
+      <c r="F32" s="18">
+        <v>0</v>
+      </c>
+      <c r="G32" s="15">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15">
+        <v>0</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="33" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" ht="18" customHeight="1">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -6988,13 +7363,23 @@
       <c r="E33" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="18"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="19"/>
+      <c r="F33" s="18">
+        <v>5</v>
+      </c>
+      <c r="G33" s="15">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15">
+        <v>0</v>
+      </c>
+      <c r="I33" s="15">
+        <v>0</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>263</v>
+      </c>
     </row>
-    <row r="34" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" ht="18" customHeight="1">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -7008,13 +7393,23 @@
       <c r="E34" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="19"/>
+      <c r="F34" s="18">
+        <v>5</v>
+      </c>
+      <c r="G34" s="15">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15">
+        <v>0</v>
+      </c>
+      <c r="I34" s="15">
+        <v>0</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>259</v>
+      </c>
     </row>
-    <row r="35" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" ht="18" customHeight="1">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -7028,13 +7423,23 @@
       <c r="E35" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="19"/>
+      <c r="F35" s="18">
+        <v>0</v>
+      </c>
+      <c r="G35" s="15">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15">
+        <v>0</v>
+      </c>
+      <c r="I35" s="15">
+        <v>0</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="18" customHeight="1">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -7060,9 +7465,11 @@
       <c r="I36" s="15">
         <v>318000</v>
       </c>
-      <c r="J36" s="19"/>
+      <c r="J36" s="19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="18" customHeight="1">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -7074,13 +7481,23 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="19"/>
+      <c r="F37" s="18">
+        <v>0</v>
+      </c>
+      <c r="G37" s="15">
+        <v>0</v>
+      </c>
+      <c r="H37" s="15">
+        <v>0</v>
+      </c>
+      <c r="I37" s="15">
+        <v>0</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>261</v>
+      </c>
     </row>
-    <row r="38" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="18" customHeight="1">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -7094,13 +7511,23 @@
       <c r="E38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="19"/>
+      <c r="F38" s="18">
+        <v>10</v>
+      </c>
+      <c r="G38" s="15">
+        <v>14000</v>
+      </c>
+      <c r="H38" s="15">
+        <v>42000</v>
+      </c>
+      <c r="I38" s="15">
+        <v>0</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>260</v>
+      </c>
     </row>
-    <row r="39" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="18" customHeight="1">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -7114,13 +7541,23 @@
       <c r="E39" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="19"/>
+      <c r="F39" s="18">
+        <v>5</v>
+      </c>
+      <c r="G39" s="15">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15">
+        <v>0</v>
+      </c>
+      <c r="I39" s="15">
+        <v>0</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="40" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="18" customHeight="1">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -7131,16 +7568,26 @@
         <v>118</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="19"/>
+      <c r="F40" s="18">
+        <v>10</v>
+      </c>
+      <c r="G40" s="15">
+        <v>24000</v>
+      </c>
+      <c r="H40" s="15">
+        <v>60000</v>
+      </c>
+      <c r="I40" s="15">
+        <v>0</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>260</v>
+      </c>
     </row>
-    <row r="41" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" ht="18" customHeight="1">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -7160,7 +7607,7 @@
       <c r="I41" s="15"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" ht="18" customHeight="1">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -7180,7 +7627,7 @@
       <c r="I42" s="15"/>
       <c r="J42" s="19"/>
     </row>
-    <row r="43" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="18" customHeight="1">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -7200,7 +7647,7 @@
       <c r="I43" s="15"/>
       <c r="J43" s="19"/>
     </row>
-    <row r="44" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="18" customHeight="1">
       <c r="A44" s="12">
         <v>43</v>
       </c>
@@ -7220,7 +7667,7 @@
       <c r="I44" s="15"/>
       <c r="J44" s="19"/>
     </row>
-    <row r="45" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="18" customHeight="1">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -7240,7 +7687,7 @@
       <c r="I45" s="15"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="18" customHeight="1">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -7260,7 +7707,7 @@
       <c r="I46" s="15"/>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="18" customHeight="1">
       <c r="A47" s="12">
         <v>46</v>
       </c>
@@ -7280,7 +7727,7 @@
       <c r="I47" s="15"/>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" ht="18" customHeight="1">
       <c r="A48" s="12">
         <v>47</v>
       </c>
@@ -7300,7 +7747,7 @@
       <c r="I48" s="15"/>
       <c r="J48" s="19"/>
     </row>
-    <row r="49" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" ht="18" customHeight="1">
       <c r="A49" s="12">
         <v>48</v>
       </c>
@@ -7320,7 +7767,7 @@
       <c r="I49" s="15"/>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" ht="18" customHeight="1">
       <c r="A50" s="12">
         <v>49</v>
       </c>
@@ -7340,7 +7787,7 @@
       <c r="I50" s="15"/>
       <c r="J50" s="19"/>
     </row>
-    <row r="51" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" ht="18" customHeight="1">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -7360,7 +7807,7 @@
       <c r="I51" s="15"/>
       <c r="J51" s="19"/>
     </row>
-    <row r="52" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" ht="18" customHeight="1">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -7380,7 +7827,7 @@
       <c r="I52" s="15"/>
       <c r="J52" s="19"/>
     </row>
-    <row r="53" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" ht="18" customHeight="1">
       <c r="A53" s="12">
         <v>52</v>
       </c>
@@ -7400,7 +7847,7 @@
       <c r="I53" s="15"/>
       <c r="J53" s="19"/>
     </row>
-    <row r="54" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" ht="18" customHeight="1">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -7420,7 +7867,7 @@
       <c r="I54" s="15"/>
       <c r="J54" s="19"/>
     </row>
-    <row r="55" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" ht="18" customHeight="1">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -7440,7 +7887,7 @@
       <c r="I55" s="15"/>
       <c r="J55" s="19"/>
     </row>
-    <row r="56" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" ht="18" customHeight="1">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -7460,7 +7907,7 @@
       <c r="I56" s="15"/>
       <c r="J56" s="19"/>
     </row>
-    <row r="57" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" ht="18" customHeight="1">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -7480,7 +7927,7 @@
       <c r="I57" s="15"/>
       <c r="J57" s="19"/>
     </row>
-    <row r="58" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" ht="18" customHeight="1">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -7500,7 +7947,7 @@
       <c r="I58" s="15"/>
       <c r="J58" s="19"/>
     </row>
-    <row r="59" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" ht="18" customHeight="1">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -7520,7 +7967,7 @@
       <c r="I59" s="15"/>
       <c r="J59" s="19"/>
     </row>
-    <row r="60" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" ht="18" customHeight="1">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -7540,7 +7987,7 @@
       <c r="I60" s="15"/>
       <c r="J60" s="19"/>
     </row>
-    <row r="61" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" ht="18" customHeight="1">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -7560,7 +8007,7 @@
       <c r="I61" s="15"/>
       <c r="J61" s="19"/>
     </row>
-    <row r="62" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" ht="18" customHeight="1">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -7580,7 +8027,7 @@
       <c r="I62" s="15"/>
       <c r="J62" s="19"/>
     </row>
-    <row r="63" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" ht="18" customHeight="1">
       <c r="A63" s="12">
         <v>62</v>
       </c>
@@ -7600,7 +8047,7 @@
       <c r="I63" s="15"/>
       <c r="J63" s="19"/>
     </row>
-    <row r="64" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:10" ht="18" customHeight="1">
       <c r="A64" s="12">
         <v>63</v>
       </c>
@@ -7620,7 +8067,7 @@
       <c r="I64" s="15"/>
       <c r="J64" s="19"/>
     </row>
-    <row r="65" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" ht="18" customHeight="1">
       <c r="A65" s="12">
         <v>64</v>
       </c>
@@ -7640,7 +8087,7 @@
       <c r="I65" s="15"/>
       <c r="J65" s="19"/>
     </row>
-    <row r="66" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" ht="18" customHeight="1">
       <c r="A66" s="12">
         <v>65</v>
       </c>
@@ -7660,7 +8107,7 @@
       <c r="I66" s="15"/>
       <c r="J66" s="19"/>
     </row>
-    <row r="67" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" ht="18" customHeight="1">
       <c r="A67" s="12">
         <v>66</v>
       </c>
@@ -7680,7 +8127,7 @@
       <c r="I67" s="15"/>
       <c r="J67" s="19"/>
     </row>
-    <row r="68" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" ht="18" customHeight="1">
       <c r="A68" s="12">
         <v>67</v>
       </c>
@@ -7700,7 +8147,7 @@
       <c r="I68" s="15"/>
       <c r="J68" s="19"/>
     </row>
-    <row r="69" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" ht="18" customHeight="1">
       <c r="A69" s="12">
         <v>68</v>
       </c>
@@ -7720,7 +8167,7 @@
       <c r="I69" s="15"/>
       <c r="J69" s="19"/>
     </row>
-    <row r="70" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" ht="18" customHeight="1">
       <c r="A70" s="12">
         <v>69</v>
       </c>
@@ -7740,7 +8187,7 @@
       <c r="I70" s="15"/>
       <c r="J70" s="19"/>
     </row>
-    <row r="71" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" ht="18" customHeight="1">
       <c r="A71" s="12">
         <v>70</v>
       </c>
@@ -7760,7 +8207,7 @@
       <c r="I71" s="15"/>
       <c r="J71" s="19"/>
     </row>
-    <row r="72" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" ht="18" customHeight="1">
       <c r="A72" s="12">
         <v>71</v>
       </c>
@@ -7780,7 +8227,7 @@
       <c r="I72" s="15"/>
       <c r="J72" s="19"/>
     </row>
-    <row r="73" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" ht="18" customHeight="1">
       <c r="A73" s="12">
         <v>72</v>
       </c>
@@ -7800,7 +8247,7 @@
       <c r="I73" s="15"/>
       <c r="J73" s="19"/>
     </row>
-    <row r="74" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" ht="18" customHeight="1">
       <c r="A74" s="12">
         <v>73</v>
       </c>
@@ -7820,7 +8267,7 @@
       <c r="I74" s="15"/>
       <c r="J74" s="19"/>
     </row>
-    <row r="75" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" ht="18" customHeight="1">
       <c r="A75" s="12">
         <v>74</v>
       </c>
@@ -7840,7 +8287,7 @@
       <c r="I75" s="15"/>
       <c r="J75" s="19"/>
     </row>
-    <row r="76" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" ht="18" customHeight="1">
       <c r="A76" s="12">
         <v>75</v>
       </c>
@@ -7860,7 +8307,7 @@
       <c r="I76" s="15"/>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" ht="18" customHeight="1">
       <c r="A77" s="12">
         <v>76</v>
       </c>
@@ -7880,7 +8327,7 @@
       <c r="I77" s="15"/>
       <c r="J77" s="19"/>
     </row>
-    <row r="78" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -7952,27 +8399,27 @@
     <hyperlink ref="E7" r:id="rId5" display="http://parsianhost.ir/" xr:uid="{57E233EE-D4D6-4F38-AD4A-E1EB18481D80}"/>
     <hyperlink ref="E8" r:id="rId6" display="http://sabtaddress.ir/" xr:uid="{62DCEF83-9646-4770-932B-B0B4F3E23D62}"/>
     <hyperlink ref="E9" r:id="rId7" display="http://asanrayaan.ir/" xr:uid="{4B6D7C6B-1F7B-4FB7-87CB-8903298FC133}"/>
-    <hyperlink ref="E10" r:id="rId8" display="http://www.takweb.ir/" xr:uid="{6E9AB595-7B69-4F24-A573-D85DA685B6CC}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{6E9AB595-7B69-4F24-A573-D85DA685B6CC}"/>
     <hyperlink ref="E11" r:id="rId9" display="http://azaronline.ir/" xr:uid="{43BC29A5-0E42-4531-AE09-7F4732BE29D1}"/>
     <hyperlink ref="E12" r:id="rId10" display="http://azaranweb.ir/" xr:uid="{607BC151-E12A-458F-8D5B-BC9F8AAD221A}"/>
     <hyperlink ref="E13" r:id="rId11" display="http://afradata.ir/" xr:uid="{3C911EA8-BB82-409C-AC81-4FDC2AAC94F1}"/>
     <hyperlink ref="E14" r:id="rId12" display="http://noornet.ir/" xr:uid="{0F5F0D8C-6DD1-4D75-9A5B-3D811C7A774E}"/>
-    <hyperlink ref="E15" r:id="rId13" display="http://www.idehnic.ir/" xr:uid="{65904291-CEAB-4231-B22A-718FDFFBF80E}"/>
-    <hyperlink ref="E16" r:id="rId14" display="http://www.datamizban.ir/" xr:uid="{0B02D814-F570-4DD9-AF6E-6F5EEE9A1EAF}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{65904291-CEAB-4231-B22A-718FDFFBF80E}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{0B02D814-F570-4DD9-AF6E-6F5EEE9A1EAF}"/>
     <hyperlink ref="E17" r:id="rId15" display="http://idehplus.ir/" xr:uid="{EAEF8EA5-DB84-437F-B9EC-D9A79D5B065D}"/>
     <hyperlink ref="E18" r:id="rId16" display="http://irpowerweb.ir/" xr:uid="{A28B473B-90EF-4877-96CC-DBCDFEF3ECF5}"/>
-    <hyperlink ref="E19" r:id="rId17" display="http://www.day.ir/" xr:uid="{50C095C0-22B2-4C8D-A8C6-4B4CAC1D01EC}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{50C095C0-22B2-4C8D-A8C6-4B4CAC1D01EC}"/>
     <hyperlink ref="E20" r:id="rId18" display="http://diyakoreseller.ir/" xr:uid="{B2156543-5519-4DAD-951D-D3E781C70E04}"/>
     <hyperlink ref="E21" r:id="rId19" display="http://novinpadideh.ir/" xr:uid="{25D977BA-51E5-4887-A897-484D6C535BA1}"/>
-    <hyperlink ref="E22" r:id="rId20" display="http://www.resellerapi.ir/" xr:uid="{95418DD6-641A-438C-A757-0F99BC168A7E}"/>
+    <hyperlink ref="E22" r:id="rId20" xr:uid="{95418DD6-641A-438C-A757-0F99BC168A7E}"/>
     <hyperlink ref="E23" r:id="rId21" display="http://webramz.ir/" xr:uid="{93DDDF5C-C105-4383-9553-2DF3E20DE0FE}"/>
     <hyperlink ref="E24" r:id="rId22" display="http://niba.ir/" xr:uid="{8AE7F955-3195-4A31-82F3-10EEE842AD31}"/>
     <hyperlink ref="E25" r:id="rId23" display="http://mihanwebhost.ir/" xr:uid="{77A2A763-FC4E-441C-89AB-89BD6A508209}"/>
     <hyperlink ref="E26" r:id="rId24" display="http://parhamreg.ir/" xr:uid="{09ADAD7B-C9DB-441A-AC34-789B2C7552BD}"/>
-    <hyperlink ref="E27" r:id="rId25" display="http://www.domainbazan.ir/" xr:uid="{C35B0161-A008-4463-8E7E-2AFC74F3025A}"/>
+    <hyperlink ref="E27" r:id="rId25" xr:uid="{C35B0161-A008-4463-8E7E-2AFC74F3025A}"/>
     <hyperlink ref="E28" r:id="rId26" display="http://spdomain.ir/" xr:uid="{51950BD9-48B8-431B-8D24-A761E4908C81}"/>
     <hyperlink ref="E29" r:id="rId27" display="http://sellir.ir/" xr:uid="{EB639299-551D-466E-9CCC-4B2A160FD110}"/>
-    <hyperlink ref="E30" r:id="rId28" display="http://www.faraso.ir/" xr:uid="{5EABF44A-59FA-4C56-916D-0C553CC3EA61}"/>
+    <hyperlink ref="E30" r:id="rId28" xr:uid="{5EABF44A-59FA-4C56-916D-0C553CC3EA61}"/>
     <hyperlink ref="E31" r:id="rId29" display="http://karait.ir/" xr:uid="{1494D3C1-8D6B-4579-9D11-3CA3D6454427}"/>
     <hyperlink ref="E32" r:id="rId30" display="http://resellha.ir/" xr:uid="{2931D0D2-39A8-421A-AE99-9917321A4D5F}"/>
     <hyperlink ref="E33" r:id="rId31" display="http://nickname.ir/" xr:uid="{A94D832F-1783-42FC-AEB4-388F6BB7C1EF}"/>
@@ -7981,7 +8428,7 @@
     <hyperlink ref="E36" r:id="rId34" display="http://jibres.ir/" xr:uid="{D6020873-348A-42CB-A4FA-E32564DEE34B}"/>
     <hyperlink ref="E38" r:id="rId35" display="http://selva.ir/" xr:uid="{0349AAC3-FE52-4F76-A228-8F7A4A582FE0}"/>
     <hyperlink ref="E39" r:id="rId36" display="http://basiscore.ir/" xr:uid="{03F0C379-8C93-41F2-BFD6-F0FB750439E9}"/>
-    <hyperlink ref="E40" r:id="rId37" display="http://www.takami.ir/" xr:uid="{3F100193-9340-4BD3-9EDB-DEF890D52088}"/>
+    <hyperlink ref="E40" r:id="rId37" xr:uid="{3F100193-9340-4BD3-9EDB-DEF890D52088}"/>
     <hyperlink ref="E41" r:id="rId38" display="http://hostpa.ir/" xr:uid="{7E21348B-648B-419F-8DD3-A24F499A278B}"/>
     <hyperlink ref="E42" r:id="rId39" display="http://meitsgroup.ir/" xr:uid="{C7715FA2-865B-49D4-A8F2-84E09237B389}"/>
     <hyperlink ref="E43" r:id="rId40" display="http://mizban.ir/" xr:uid="{394551FD-A1F0-479E-A9C4-01317B54327E}"/>
@@ -8054,17 +8501,17 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>239</v>
       </c>
@@ -8075,7 +8522,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11">
       <c r="A2" s="16">
         <v>44657</v>
       </c>
@@ -8086,21 +8533,24 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="K3" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" x14ac:dyDescent="0.4">
-      <c r="K4" s="1" t="s">
+    <row r="4" spans="1:11">
+      <c r="K4" s="20" t="s">
         <v>237</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{73B2A577-E110-4422-96FF-17CF77DD00DC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>